<commit_message>
Started wiring components in Quartus
</commit_message>
<xml_diff>
--- a/Final_Task_3_Resources.xlsx
+++ b/Final_Task_3_Resources.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>MATLab Function</t>
   </si>
@@ -59,10 +59,13 @@
     <t>Madgwick_update</t>
   </si>
   <si>
-    <t>Optimizations Used:</t>
-  </si>
-  <si>
-    <t>Register Inputs (for pipelining)</t>
+    <t>Register Inputs</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -150,38 +153,41 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -191,20 +197,28 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -488,233 +502,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="12.7109375" customWidth="1"/>
+    <col min="2" max="11" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
         <v>4</v>
       </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E4" s="1">
         <v>6</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
         <v>10</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H4" s="1">
         <v>124</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I4" s="1">
         <v>49</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J4" s="1">
         <v>8</v>
       </c>
-      <c r="I3" s="1">
+      <c r="K4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F5" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
         <v>133</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I5" s="1">
         <v>133</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J5" s="1">
         <v>8</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K5" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
         <v>55</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
         <v>20</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
         <v>734</v>
       </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
         <v>35</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E8" s="1">
         <v>6</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1">
         <v>28</v>
       </c>
-      <c r="F7" s="1">
+      <c r="H8" s="1">
         <v>12</v>
       </c>
-      <c r="G7" s="1">
+      <c r="I8" s="1">
         <v>361</v>
       </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="4">
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>

</xml_diff>